<commit_message>
add import value validation
</commit_message>
<xml_diff>
--- a/DataPortalCare/src/test/resources/ProofExampleWrongValues.xlsx
+++ b/DataPortalCare/src/test/resources/ProofExampleWrongValues.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>Station</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>sdd</t>
+  </si>
+  <si>
+    <t>Nacht</t>
   </si>
 </sst>
 </file>
@@ -460,10 +463,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,6 +560,44 @@
         <v>1.5</v>
       </c>
     </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="5">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="4">
+        <v>35</v>
+      </c>
+      <c r="I3" s="1">
+        <v>2344</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1.5678000000000001</v>
+      </c>
+      <c r="K3" s="1">
+        <v>42.548999999999999</v>
+      </c>
+      <c r="L3" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="74" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>